<commit_message>
[expression] - [CSV expression]: fix issue dealing with content that contains delimiter or double quotes.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_expressions.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_expressions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFC7A07-4EEF-E640-A8DB-48D402CFAED3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DB3670-5C16-4740-A803-3B6AC3DF6309}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4560" windowWidth="40960" windowHeight="21040" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="57600" windowHeight="17760" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -2059,14 +2059,6 @@
     <t>[TEXT(${expected}) =&gt; text]</t>
   </si>
   <si>
-    <t>[CSV(${initial}) =&gt; 
- parse(header=true) 
- replaceColumnRegex(^([^"\].*[^"\]\)$,"$1",*)
- replaceColumnRegex("null",null,*) 
- text
-]</t>
-  </si>
-  <si>
     <t>clear(variables)</t>
   </si>
   <si>
@@ -2092,6 +2084,14 @@
   </si>
   <si>
     <t>2ND UNIT,AMORT-SERIES,ART DEPT,ASSET SALE / OTHER REVENUE,ATL TRAVEL &amp; LIVING,BOTTLE SHOW CREDIT,BTL TRAVEL &amp; LIVING,CAMERA,COSTUMES,DIRECTOR,EDITORIAL,EXTRAS,FACILITY/STAGE COSTS,GENERAL EXPENSE,GRIP/SET OPERATIONS,INSURANCE,LOCATION &amp; OFFICE EXPENSE,MAKEUP / HAIR,MUSIC,PACKAGE FEE,PIC VEHICLES/ANIMALS/HANDLERS,POST PRODUCTION FILM &amp; LAB,POST PRODUCTION SOUND,PRODUCER,PRODUCTION SOUND,PRODUCTION STAFF,PRODUCTION STOCK &amp; LAB,PROPS,PUBLICITY,RESIDUALS,SET CONSTRUCTION,SET DRESSING,SET LIGHTING,SPECIAL FX,STRIKE,TALENT,TESTS,TITLES,TRANSPORTATION,VISUAL EFFECTS,WRITERS</t>
+  </si>
+  <si>
+    <t>[CSV(${initial}) =&gt; 
+ parse(header=true,keepQuote=true) 
+ replaceColumnRegex(^([^"\].*[^"\]\)$,"$1",*)
+ replaceColumnRegex("null",null,*) 
+ text
+]</t>
   </si>
 </sst>
 </file>
@@ -2368,6 +2368,9 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -2395,9 +2398,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3770,7 +3770,7 @@
         <v>52</v>
       </c>
       <c r="F18" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="H18" t="s">
         <v>89</v>
@@ -3839,7 +3839,7 @@
         <v>294</v>
       </c>
       <c r="L21" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="Z21" t="s">
         <v>107</v>
@@ -4810,12 +4810,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="24" t="s">
         <v>11</v>
       </c>
@@ -4833,20 +4833,20 @@
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="38"/>
     </row>
     <row r="2" spans="1:15" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
       <c r="E2" s="25"/>
       <c r="F2" s="26"/>
       <c r="G2" s="25"/>
@@ -4856,10 +4856,10 @@
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
@@ -16349,7 +16349,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="108" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16371,12 +16371,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="31" t="s">
         <v>11</v>
       </c>
@@ -16394,20 +16394,20 @@
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="38"/>
     </row>
     <row r="2" spans="1:15" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
       <c r="E2" s="25"/>
       <c r="F2" s="26"/>
       <c r="G2" s="25"/>
@@ -16417,10 +16417,10 @@
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
@@ -16536,7 +16536,7 @@
       <c r="N6" s="15"/>
       <c r="O6" s="3"/>
     </row>
-    <row r="7" spans="1:15" ht="112" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
       <c r="B7" s="5"/>
       <c r="C7" s="13" t="s">
@@ -16549,7 +16549,7 @@
         <v>596</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>603</v>
+        <v>610</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -16588,7 +16588,7 @@
     </row>
     <row r="9" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="14" t="s">
@@ -16598,7 +16598,7 @@
         <v>315</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -16618,14 +16618,14 @@
       <c r="D10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="40" t="s">
-        <v>610</v>
+      <c r="E10" s="32" t="s">
+        <v>609</v>
       </c>
       <c r="F10" s="23" t="s">
+        <v>606</v>
+      </c>
+      <c r="G10" s="10" t="s">
         <v>607</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>608</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -33011,7 +33011,7 @@
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C8 C11:C700" xr:uid="{CF1C1FAC-1EBE-8345-BF66-48D147E1AFD3}">
       <formula1>target</formula1>
     </dataValidation>
@@ -33052,12 +33052,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="29" t="s">
         <v>11</v>
       </c>
@@ -33075,20 +33075,20 @@
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="38"/>
     </row>
     <row r="2" spans="1:15" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
       <c r="E2" s="25"/>
       <c r="F2" s="26"/>
       <c r="G2" s="25"/>
@@ -33098,10 +33098,10 @@
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
@@ -44595,12 +44595,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="30" t="s">
         <v>11</v>
       </c>
@@ -44618,20 +44618,20 @@
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="38"/>
     </row>
     <row r="2" spans="1:15" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
       <c r="E2" s="25"/>
       <c r="F2" s="26"/>
       <c r="G2" s="25"/>
@@ -44641,10 +44641,10 @@
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>

</xml_diff>